<commit_message>
update le journal de travail
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail.xlsx
+++ b/Documentation/Journal de travail.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10522"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D2FD24A5-3E96-2749-9C4A-7E12C059FC4F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,29 +20,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Journal de travail</t>
   </si>
   <si>
-    <t>Projet Tech</t>
-  </si>
-  <si>
-    <t>Application de recherche de fichier</t>
-  </si>
-  <si>
     <t>Auteur</t>
   </si>
   <si>
-    <t>Quentin Rossier  Si-T1a</t>
-  </si>
-  <si>
     <t>Durée</t>
   </si>
   <si>
-    <t>31.08.2018 - 14.12.2018</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -66,36 +55,12 @@
     <t>Création du github</t>
   </si>
   <si>
-    <t>Recherche de sit web sur des quizz</t>
-  </si>
-  <si>
-    <t>Groupe avec sacha</t>
-  </si>
-  <si>
     <t>Lecture de documentation sur les quizz</t>
   </si>
   <si>
-    <t>Discussion avec Sasha sur le travail à fournir aujourd'hui</t>
-  </si>
-  <si>
-    <t>Analyse d'un site QCM</t>
-  </si>
-  <si>
     <t>Semaine 2</t>
   </si>
   <si>
-    <t>Analyse d'un autre site de QCM</t>
-  </si>
-  <si>
-    <t>Githbub + Journal de bord</t>
-  </si>
-  <si>
-    <t>qcmweb.fr</t>
-  </si>
-  <si>
-    <t>targetweb.fr</t>
-  </si>
-  <si>
     <t>Semaine 3</t>
   </si>
   <si>
@@ -127,12 +92,45 @@
   </si>
   <si>
     <t xml:space="preserve">documentation de mise en place pas très claire ( bug?) affichage d'une page par-dessus l'autre </t>
+  </si>
+  <si>
+    <t>Jérémy Gfeller &amp; Senistan Jegarajasingam</t>
+  </si>
+  <si>
+    <t>10.12.2018 - 01.02.2019</t>
+  </si>
+  <si>
+    <t>Groupe avec senistan</t>
+  </si>
+  <si>
+    <t>Recherche de sites web à comparer</t>
+  </si>
+  <si>
+    <t>Projet</t>
+  </si>
+  <si>
+    <t>Vue.js - création d'un quizz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analyse de plusieurs sites </t>
+  </si>
+  <si>
+    <t>Quizlet, Quipo Quiz, Quizz.fr</t>
+  </si>
+  <si>
+    <t>Trouver trois tamplates pertinants</t>
+  </si>
+  <si>
+    <t>Création du moodboard</t>
+  </si>
+  <si>
+    <t>Tirer la sythèse pour la partie analyse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -172,7 +170,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -352,13 +350,44 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -394,20 +423,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -431,10 +450,19 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -452,9 +480,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -472,6 +497,14 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -752,407 +785,354 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="63.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="63.33203125" customWidth="1"/>
     <col min="4" max="4" width="54" customWidth="1"/>
-    <col min="5" max="5" width="50.85546875" customWidth="1"/>
+    <col min="5" max="5" width="50.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="40"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="38"/>
       <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="39"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="41"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="E2" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="D3" s="6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="10" t="s">
+      <c r="B7" s="13">
+        <f>SUM(B8:B12)</f>
+        <v>0.15625</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="35"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="28">
+        <v>43444</v>
+      </c>
+      <c r="B8" s="20">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>9</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="13">
-        <f>SUM(B8:B15)</f>
-        <v>0.15625</v>
-      </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="36"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="30">
-        <v>43444</v>
-      </c>
-      <c r="B8" s="24">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>13</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="16" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="29"/>
+      <c r="B9" s="21">
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="16"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="26">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="29"/>
+      <c r="B10" s="22">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="16"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
-      <c r="B11" s="27">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="30"/>
+      <c r="B11" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="17"/>
+    </row>
+    <row r="12" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="26">
+        <v>43446</v>
+      </c>
+      <c r="B12" s="19">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="13">
+        <f>SUM(B14:B16)</f>
+        <v>0.15625</v>
+      </c>
+      <c r="C13" s="33"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="35"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="28">
+        <v>43451</v>
+      </c>
+      <c r="B14" s="14">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="29"/>
+      <c r="B15" s="14">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="15"/>
+      <c r="E15" s="16"/>
+    </row>
+    <row r="16" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="27">
+        <v>43453</v>
+      </c>
+      <c r="B16" s="45">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="43"/>
+      <c r="E16" s="44"/>
+    </row>
+    <row r="17" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="13">
+        <f>SUM(B18:B22)</f>
+        <v>0.15625</v>
+      </c>
+      <c r="C17" s="33"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="35"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="28">
+        <v>43472</v>
+      </c>
+      <c r="B18" s="19">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="29"/>
+      <c r="B19" s="19">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="29"/>
+      <c r="B20" s="19">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="31">
+        <v>43474</v>
+      </c>
+      <c r="B21" s="19">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C21" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="20"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="31">
-        <v>43446</v>
-      </c>
-      <c r="B12" s="23">
-        <v>3.472222222222222E-3</v>
-      </c>
-      <c r="C12" s="15" t="s">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="29"/>
+      <c r="B22" s="19">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C22" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
-      <c r="B13" s="23">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="C13" s="15" t="s">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="29"/>
+      <c r="B23" s="19"/>
+    </row>
+    <row r="24" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="32"/>
+      <c r="B24" s="19"/>
+    </row>
+    <row r="25" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
         <v>19</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="B14" s="23">
-        <v>2.4305555555555556E-2</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="31"/>
-      <c r="B15" s="23">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="13">
-        <f>SUM(B17:B24)</f>
-        <v>0</v>
-      </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="36"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="30">
-        <v>43444</v>
-      </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="16"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="16"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="16"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="37"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="20"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="32">
-        <v>43446</v>
-      </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="15"/>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="15"/>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="15"/>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="33"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="15"/>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
-        <v>25</v>
       </c>
       <c r="B25" s="13">
         <f>SUM(B26:B30)</f>
-        <v>0.15625</v>
-      </c>
-      <c r="C25" s="34"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="36"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="30">
-        <v>43472</v>
-      </c>
-      <c r="B26" s="23">
-        <v>3.125E-2</v>
-      </c>
-      <c r="C26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
-      <c r="B27" s="23">
-        <v>3.125E-2</v>
+        <v>9.375E-2</v>
+      </c>
+      <c r="C25" s="33"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="35"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="28">
+        <v>43479</v>
+      </c>
+      <c r="B26" s="25">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="29"/>
+      <c r="B27" s="19">
+        <v>2.4305555555555556E-2</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
-      <c r="B28" s="23">
-        <v>3.125E-2</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A28" s="29"/>
+      <c r="B28" s="19">
+        <v>6.25E-2</v>
       </c>
       <c r="C28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="32">
+        <v>22</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="31">
         <v>43474</v>
       </c>
-      <c r="B29" s="23">
-        <v>3.125E-2</v>
-      </c>
-      <c r="C29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="31"/>
-      <c r="B30" s="23">
-        <v>3.125E-2</v>
-      </c>
-      <c r="C30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
-      <c r="B31" s="23"/>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="33"/>
-      <c r="B32" s="23"/>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="13">
-        <f>SUM(B34:B38)</f>
-        <v>9.375E-2</v>
-      </c>
-      <c r="C33" s="34"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="36"/>
-    </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="30">
-        <v>43479</v>
-      </c>
-      <c r="B34" s="29">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="C34" s="28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
-      <c r="B35" s="23">
-        <v>2.4305555555555556E-2</v>
-      </c>
-      <c r="C35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
-      <c r="B36" s="23">
-        <v>6.25E-2</v>
-      </c>
-      <c r="C36" t="s">
-        <v>34</v>
-      </c>
-      <c r="D36" s="28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="32">
-        <v>43474</v>
-      </c>
-      <c r="B37" s="23"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="31"/>
-      <c r="B38" s="23"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
-      <c r="B39" s="23"/>
-    </row>
-    <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="33"/>
-      <c r="B40" s="23"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="23"/>
+      <c r="B29" s="19"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="29"/>
+      <c r="B30" s="19"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="29"/>
+      <c r="B31" s="19"/>
+    </row>
+    <row r="32" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="32"/>
+      <c r="B32" s="19"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A17:A20"/>
+  <mergeCells count="11">
+    <mergeCell ref="A18:A20"/>
     <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A26:A28"/>
     <mergeCell ref="C25:E25"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="C17:E17"/>
     <mergeCell ref="A1:C2"/>
     <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="C13:E13"/>
     <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="C33:E33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Journal de travail à jour
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail.xlsx
+++ b/Documentation/Journal de travail.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10522"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D2FD24A5-3E96-2749-9C4A-7E12C059FC4F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F455D0E5-9A53-3D43-B098-17B9DD58E8EF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -64,36 +64,12 @@
     <t>Semaine 3</t>
   </si>
   <si>
-    <t>Recherche et analyse de template</t>
-  </si>
-  <si>
-    <t>Prise de matériel pour le moonboard et création de celui-ci</t>
-  </si>
-  <si>
-    <t>Maquette, page web crée</t>
-  </si>
-  <si>
-    <t>Finir la maquette mokupe</t>
-  </si>
-  <si>
-    <t>tuto quizz vujs</t>
-  </si>
-  <si>
     <t>Semaine 4</t>
   </si>
   <si>
-    <t>Discussion avec Sasha sur le choix de la templat et du design des maquettes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Finition du tutoriel de quiz </t>
   </si>
   <si>
-    <t>Installation et compréhension de la template Aragon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentation de mise en place pas très claire ( bug?) affichage d'une page par-dessus l'autre </t>
-  </si>
-  <si>
     <t>Jérémy Gfeller &amp; Senistan Jegarajasingam</t>
   </si>
   <si>
@@ -125,6 +101,33 @@
   </si>
   <si>
     <t>Tirer la sythèse pour la partie analyse</t>
+  </si>
+  <si>
+    <t>Semaine 5</t>
+  </si>
+  <si>
+    <t>Création du zooning et wireframe partie 1</t>
+  </si>
+  <si>
+    <t>Création du zooning et wireframe partie 2</t>
+  </si>
+  <si>
+    <t>Création de la page de réponse sur photoshop</t>
+  </si>
+  <si>
+    <t>Création du document de mise en globale</t>
+  </si>
+  <si>
+    <t>Tuto Vue js</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Montrer à Senistan ce qui a été fait dans la partie conception </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajouter les pages inscription et connexion à ce qu'a fait Senistan </t>
+  </si>
+  <si>
+    <t>Modifier le template du site complet pour faire la même chose que sur les maquettes</t>
   </si>
 </sst>
 </file>
@@ -170,7 +173,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -375,6 +378,32 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -387,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -459,43 +488,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -503,9 +496,56 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="113" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -802,27 +842,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="38"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="37"/>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="41"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="40"/>
       <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -832,7 +872,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -868,12 +908,12 @@
         <f>SUM(B8:B12)</f>
         <v>0.15625</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="35"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="44"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="28">
+      <c r="A8" s="33">
         <v>43444</v>
       </c>
       <c r="B8" s="20">
@@ -884,14 +924,14 @@
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="16" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="29"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="21">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -902,18 +942,18 @@
       <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="29"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="22">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="16"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="30"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -931,10 +971,10 @@
         <v>6.25E-2</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -945,30 +985,30 @@
         <f>SUM(B14:B16)</f>
         <v>0.15625</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="35"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="44"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="28">
+      <c r="A14" s="33">
         <v>43451</v>
       </c>
       <c r="B14" s="14">
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="16"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="29"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="14">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="16"/>
@@ -980,159 +1020,166 @@
       <c r="B16" s="45">
         <v>6.25E-2</v>
       </c>
-      <c r="C16" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="43"/>
-      <c r="E16" s="44"/>
+      <c r="C16" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="31"/>
+      <c r="E16" s="32"/>
     </row>
     <row r="17" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="13">
-        <f>SUM(B18:B22)</f>
+      <c r="B17" s="46">
+        <f>SUM(B18:B19)</f>
         <v>0.15625</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="35"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="44"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="28">
         <v>43472</v>
       </c>
       <c r="B18" s="19">
+        <v>9.375E-2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="47">
+        <v>43474</v>
+      </c>
+      <c r="B19" s="48">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C19" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="31"/>
+      <c r="E19" s="32"/>
+    </row>
+    <row r="20" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="13">
+        <f>SUM(B21:B23)</f>
+        <v>0.15625</v>
+      </c>
+      <c r="C20" s="42"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="44"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="33">
+        <v>43479</v>
+      </c>
+      <c r="B21" s="25">
         <v>3.125E-2</v>
       </c>
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="29"/>
-      <c r="B19" s="19">
-        <v>3.125E-2</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="C21" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="34"/>
+      <c r="B22" s="19">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="29">
+        <v>43481</v>
+      </c>
+      <c r="B23" s="19">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="31"/>
+      <c r="E23" s="32"/>
+    </row>
+    <row r="24" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="13">
+        <f>SUM(B25:B28)</f>
+        <v>0.17708333333333334</v>
+      </c>
+      <c r="C24" s="42"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="44"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="33">
+        <v>43486</v>
+      </c>
+      <c r="B25" s="25">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="34"/>
+      <c r="B26" s="19">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="C26" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="29"/>
-      <c r="B20" s="19">
-        <v>3.125E-2</v>
-      </c>
-      <c r="C20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="31">
-        <v>43474</v>
-      </c>
-      <c r="B21" s="19">
-        <v>3.125E-2</v>
-      </c>
-      <c r="C21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="29"/>
-      <c r="B22" s="19">
-        <v>3.125E-2</v>
-      </c>
-      <c r="C22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="29"/>
-      <c r="B23" s="19"/>
-    </row>
-    <row r="24" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
-      <c r="B24" s="19"/>
-    </row>
-    <row r="25" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="13">
-        <f>SUM(B26:B30)</f>
-        <v>9.375E-2</v>
-      </c>
-      <c r="C25" s="33"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="35"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="28">
-        <v>43479</v>
-      </c>
-      <c r="B26" s="25">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="C26" s="24" t="s">
-        <v>20</v>
-      </c>
+      <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="29"/>
+      <c r="A27" s="34"/>
       <c r="B27" s="19">
-        <v>2.4305555555555556E-2</v>
+        <v>7.2916666666666671E-2</v>
       </c>
       <c r="C27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A28" s="29"/>
-      <c r="B28" s="19">
+        <v>34</v>
+      </c>
+      <c r="D27" s="24"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="47">
+        <v>43488</v>
+      </c>
+      <c r="B28" s="48">
         <v>6.25E-2</v>
       </c>
-      <c r="C28" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="31">
-        <v>43474</v>
-      </c>
-      <c r="B29" s="19"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="29"/>
-      <c r="B30" s="19"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="29"/>
-      <c r="B31" s="19"/>
-    </row>
-    <row r="32" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
-      <c r="B32" s="19"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="19"/>
+      <c r="C28" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="49"/>
+      <c r="E28" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="C25:E25"/>
+  <mergeCells count="10">
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="A25:A27"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="A1:C2"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="C20:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>